<commit_message>
Final Commit and Code Changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\ECommerce_Web_Automation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium_Automation\ECommerce_Web_Automation_TestNG\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0F6687-891A-4C15-9D07-FA4D8DC13CBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF006EC-2061-43A7-9DEE-A14FFA312A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{32D22023-B6D0-44C0-A8C8-42184FF9CF80}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{32D22023-B6D0-44C0-A8C8-42184FF9CF80}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageTest" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>UserName</t>
   </si>
@@ -117,6 +116,9 @@
   </si>
   <si>
     <t>In stock</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -176,10 +178,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,13 +504,13 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -523,7 +526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -546,16 +549,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.21875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -572,7 +575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -599,16 +602,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -616,7 +619,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -633,18 +636,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9712D72A-33CC-4DC2-8AAE-295ABB60E5A2}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -658,7 +661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -668,12 +671,13 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -681,20 +685,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F81152AF-DAAD-4A97-944F-7F11B2E27E1B}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -711,7 +715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Committing the latest code
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium_Automation\ECommerce_Web_Automation_TestNG\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF006EC-2061-43A7-9DEE-A14FFA312A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2F5E5D-88F3-40C0-9455-BE4E18313FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{32D22023-B6D0-44C0-A8C8-42184FF9CF80}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="7" xr2:uid="{32D22023-B6D0-44C0-A8C8-42184FF9CF80}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageTest" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="ProductDetailsPageTest" sheetId="3" r:id="rId3"/>
     <sheet name="ShoppingCartPageTest" sheetId="4" r:id="rId4"/>
     <sheet name="OrderDetailsPageTest" sheetId="5" r:id="rId5"/>
+    <sheet name="OrderShippingPageTest" sheetId="6" r:id="rId6"/>
+    <sheet name="OrderPaymentPageTest" sheetId="7" r:id="rId7"/>
+    <sheet name="OrderConfirmationPageTest" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>UserName</t>
   </si>
@@ -119,6 +122,42 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>PaymentMode</t>
+  </si>
+  <si>
+    <t>You have chosen to pay by check. Here is a short summary of your order:</t>
+  </si>
+  <si>
+    <t>PaymentText</t>
+  </si>
+  <si>
+    <t>TotalAmountOfProduct</t>
+  </si>
+  <si>
+    <t>CHECK PAYMENT</t>
+  </si>
+  <si>
+    <t>$18.51</t>
+  </si>
+  <si>
+    <t>ORDER CONFIRMATION</t>
+  </si>
+  <si>
+    <t>Your order on My Store is complete.</t>
+  </si>
+  <si>
+    <t>Your order will be sent as soon as we receive your payment.</t>
+  </si>
+  <si>
+    <t>OrderConfimationPageLabel</t>
+  </si>
+  <si>
+    <t>OrderConfimationSuccessMessage</t>
+  </si>
+  <si>
+    <t>OrderConfirmationText</t>
   </si>
 </sst>
 </file>
@@ -178,11 +217,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -636,7 +676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9712D72A-33CC-4DC2-8AAE-295ABB60E5A2}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -686,7 +726,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,4 +775,154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F354FFD-1442-4675-ACA2-0E70B911F2DC}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F45B90-3F66-4C88-9FF3-1DBABE4DF64C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E059EA69-26F2-49AB-8EA0-BB88D203D3B0}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>